<commit_message>
swapped xy vals and updated colorLayout
</commit_message>
<xml_diff>
--- a/ClueInitFiles/data/ClueLayoutColor.xlsx
+++ b/ClueInitFiles/data/ClueLayoutColor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\eclipse-workspace\ClueGame\ClueInitFiles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8F7DEF4E-D267-4822-9CAE-5FDC58521DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C88E7719-E123-4305-9D44-2A021DF89528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25800" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{4E7ECD27-46A9-4881-883E-5276EA3726F4}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="50">
   <si>
     <t>X</t>
   </si>
@@ -94,9 +94,6 @@
     <t>C#</t>
   </si>
   <si>
-    <t>C*</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -158,6 +155,21 @@
   </si>
   <si>
     <t xml:space="preserve">Adjacen twalkways </t>
+  </si>
+  <si>
+    <t>W&lt; (red)</t>
+  </si>
+  <si>
+    <t>Test Targets</t>
+  </si>
+  <si>
+    <t>Test Occupied</t>
+  </si>
+  <si>
+    <t>C*(Black)</t>
+  </si>
+  <si>
+    <t>&lt;&lt;===</t>
   </si>
 </sst>
 </file>
@@ -313,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,6 +559,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -708,7 +732,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -730,6 +754,11 @@
     <xf numFmtId="0" fontId="8" fillId="40" borderId="0" xfId="8" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="43" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1108,7 +1137,7 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V32" sqref="V32"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="AE2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
@@ -1392,7 +1421,7 @@
         <v>2</v>
       </c>
       <c r="AE3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
@@ -1490,7 +1519,7 @@
         <v>3</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AF4" s="8"/>
       <c r="AG4" s="8"/>
@@ -1588,7 +1617,7 @@
         <v>4</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
@@ -1686,7 +1715,7 @@
         <v>5</v>
       </c>
       <c r="AE6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
@@ -1784,7 +1813,7 @@
         <v>6</v>
       </c>
       <c r="AE7" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AF7" s="17"/>
       <c r="AG7" s="17"/>
@@ -1881,7 +1910,7 @@
         <v>7</v>
       </c>
       <c r="AE8" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF8" s="20"/>
       <c r="AG8" s="20"/>
@@ -1977,6 +2006,11 @@
       <c r="AD9" s="10">
         <v>8</v>
       </c>
+      <c r="AE9" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -2069,6 +2103,11 @@
       <c r="AD10" s="10">
         <v>9</v>
       </c>
+      <c r="AE10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -2448,7 +2487,7 @@
       <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="23" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -2553,7 +2592,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>10</v>
@@ -3045,7 +3084,7 @@
       <c r="R21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S21" s="5" t="s">
+      <c r="S21" s="25" t="s">
         <v>11</v>
       </c>
       <c r="T21" s="3" t="s">
@@ -3064,10 +3103,10 @@
         <v>22</v>
       </c>
       <c r="Y21" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z21" s="3" t="s">
-        <v>22</v>
+        <v>48</v>
+      </c>
+      <c r="Z21" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="AA21" s="3" t="s">
         <v>22</v>
@@ -3101,7 +3140,7 @@
       <c r="F22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="25" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="5" t="s">
@@ -3274,13 +3313,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -3363,19 +3402,19 @@
         <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -3452,25 +3491,25 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>10</v>
@@ -3544,25 +3583,25 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>13</v>
@@ -3636,25 +3675,25 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>10</v>
@@ -3731,19 +3770,19 @@
         <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>10</v>
@@ -3826,13 +3865,13 @@
         <v>0</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>10</v>
@@ -4262,7 +4301,7 @@
       <c r="Y34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Z34" s="5" t="s">
+      <c r="Z34" s="22" t="s">
         <v>20</v>
       </c>
       <c r="AA34" s="1" t="s">
@@ -4286,79 +4325,79 @@
         <v>0</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="O35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="P35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N35" s="3" t="s">
+      <c r="Q35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="S35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="V35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O35" s="3" t="s">
+      <c r="Z35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P35" s="3" t="s">
+      <c r="AA35" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Q35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="X35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y35" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z35" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA35" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="AB35" s="1" t="s">
         <v>0</v>
@@ -4375,85 +4414,85 @@
         <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="N36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="O36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="P36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="Q36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M36" s="3" t="s">
+      <c r="R36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N36" s="3" t="s">
+      <c r="Y36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O36" s="3" t="s">
+      <c r="Z36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P36" s="3" t="s">
+      <c r="AA36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q36" s="3" t="s">
+      <c r="AB36" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="R36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="X36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB36" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="AC36" s="1" t="s">
         <v>0</v>
@@ -4464,91 +4503,91 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="M37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="N37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="O37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="P37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="Q37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L37" s="3" t="s">
+      <c r="R37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="V37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M37" s="3" t="s">
+      <c r="X37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N37" s="3" t="s">
+      <c r="Y37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O37" s="3" t="s">
+      <c r="Z37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P37" s="3" t="s">
+      <c r="AA37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="3" t="s">
+      <c r="AB37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R37" s="3" t="s">
+      <c r="AC37" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="S37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="X37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC37" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="AD37" s="10">
         <v>36</v>
@@ -4556,25 +4595,25 @@
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>10</v>
@@ -4589,25 +4628,25 @@
         <v>11</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S38" s="9" t="s">
         <v>13</v>
@@ -4622,25 +4661,25 @@
         <v>10</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y38" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z38" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="Z38" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="AA38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AB38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AC38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AD38" s="10">
         <v>37</v>
@@ -4648,91 +4687,91 @@
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="M39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="N39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="O39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="P39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="R39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L39" s="3" t="s">
+      <c r="S39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M39" s="3" t="s">
+      <c r="X39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N39" s="3" t="s">
+      <c r="Y39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O39" s="3" t="s">
+      <c r="Z39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P39" s="3" t="s">
+      <c r="AA39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q39" s="3" t="s">
+      <c r="AB39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R39" s="3" t="s">
+      <c r="AC39" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="S39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="X39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC39" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="AD39" s="10">
         <v>38</v>
@@ -4743,85 +4782,85 @@
         <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="N40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="O40" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="P40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="Q40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M40" s="3" t="s">
+      <c r="R40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N40" s="3" t="s">
+      <c r="Y40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O40" s="3" t="s">
+      <c r="Z40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P40" s="3" t="s">
+      <c r="AA40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q40" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X40" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y40" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z40" s="3" t="s">
+      <c r="AB40" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="AA40" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB40" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="AC40" s="1" t="s">
         <v>0</v>
@@ -4838,79 +4877,79 @@
         <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="O41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="P41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N41" s="3" t="s">
+      <c r="Q41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O41" s="3" t="s">
+      <c r="Z41" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P41" s="3" t="s">
+      <c r="AA41" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="T41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="W41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z41" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA41" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="AB41" s="1" t="s">
         <v>0</v>

</xml_diff>